<commit_message>
se ajustan casos de prueba en la vista visor informacion tecnica red y documentacion
</commit_message>
<xml_diff>
--- a/docs/test-cases/visorInformacionTecnicaRed.xlsx
+++ b/docs/test-cases/visorInformacionTecnicaRed.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDD6DB6-AC7B-4E86-B1BB-83C545F1093C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>ID Caso</t>
   </si>
@@ -94,13 +93,31 @@
   </si>
   <si>
     <t>CP_INFTECRED_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtro de búsqueda </t>
+  </si>
+  <si>
+    <t>Haber ingresado a la vista y dado clic botón de mostrar filtro</t>
+  </si>
+  <si>
+    <t>CP_INFTECRED_003</t>
+  </si>
+  <si>
+    <t>Ver dispostivos</t>
+  </si>
+  <si>
+    <t>CP_INFTECRED_004</t>
+  </si>
+  <si>
+    <t>Editar estado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +138,14 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -181,11 +206,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -202,6 +264,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,16 +557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
@@ -504,7 +580,7 @@
     <col min="12" max="12" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +618,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="120">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -580,23 +656,71 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="84.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="57" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" ht="55.5" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="E7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>